<commit_message>
getting new branch onto github
</commit_message>
<xml_diff>
--- a/resources/ResourceFile_Depression_nov19.xlsx
+++ b/resources/ResourceFile_Depression_nov19.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andrew Phillips\Dropbox\Thanzi la Onse\04 - Methods Repository\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andrew Phillips\PycharmProjects\TLOmodel\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -2174,7 +2174,7 @@
         <xdr:cNvPr id="2" name="TextBox 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2241,7 +2241,7 @@
         <xdr:cNvPr id="3" name="TextBox 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2325,7 +2325,7 @@
         <xdr:cNvPr id="38" name="Picture 37">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000026000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000026000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2369,7 +2369,7 @@
         <xdr:cNvPr id="5" name="Picture 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000005000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2456,7 +2456,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0B00-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0B00-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2517,7 +2517,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0B00-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0B00-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2578,7 +2578,7 @@
         <xdr:cNvPr id="4" name="Picture 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0B00-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0B00-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2639,7 +2639,7 @@
         <xdr:cNvPr id="5" name="Picture 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0B00-000005000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0B00-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2700,7 +2700,7 @@
         <xdr:cNvPr id="6" name="Picture 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0B00-000006000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0B00-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2761,7 +2761,7 @@
         <xdr:cNvPr id="7" name="Picture 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0B00-000007000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0B00-000007000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2822,7 +2822,7 @@
         <xdr:cNvPr id="8" name="Picture 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0B00-000008000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0B00-000008000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5793,7 +5793,7 @@
   <dimension ref="A1:H33"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -5923,7 +5923,7 @@
         <v>551</v>
       </c>
       <c r="B15">
-        <v>1.8E-3</v>
+        <v>2.0999999999999999E-3</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">

</xml_diff>